<commit_message>
Test - user can register ONLY with valid e-mail
</commit_message>
<xml_diff>
--- a/data/ProjekatData.xlsx
+++ b/data/ProjekatData.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="19155" windowHeight="11820" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="19155" windowHeight="11820" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Plan" sheetId="1" r:id="rId1"/>
-    <sheet name="TC Reg1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="TestPlan" sheetId="1" r:id="rId1"/>
+    <sheet name="TCReg1" sheetId="2" r:id="rId2"/>
+    <sheet name="TCReg2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>Section</t>
   </si>
@@ -85,13 +85,55 @@
   </si>
   <si>
     <t>Authentication page is opened</t>
+  </si>
+  <si>
+    <t>TC Reg2</t>
+  </si>
+  <si>
+    <t>Verify that user can register using only valid email adress</t>
+  </si>
+  <si>
+    <t>Enter invalid e-mail address</t>
+  </si>
+  <si>
+    <t>pera#gmail.com</t>
+  </si>
+  <si>
+    <t>E-mail is entered and visible</t>
+  </si>
+  <si>
+    <t>Click "Create an account button"</t>
+  </si>
+  <si>
+    <t>User can`t registrer with invalid e-mail. Error message: "Invalid email address." is displayed.</t>
+  </si>
+  <si>
+    <t>Refresh page</t>
+  </si>
+  <si>
+    <t>Page is refreshed, error message is dissapeared. E-mail field is empty and ready for entering an e-mail.</t>
+  </si>
+  <si>
+    <t>pera@gmail.com</t>
+  </si>
+  <si>
+    <t>Enter valid e-mail address (for next text enter e-mail in format pera+n@gmail.com…n = 1, 2, 3...)</t>
+  </si>
+  <si>
+    <t>TCReg1</t>
+  </si>
+  <si>
+    <t>TCReg2</t>
+  </si>
+  <si>
+    <t>E-mail is accepted, and user is forwarded to "CREATE AN ACCOUNT"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +148,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -159,10 +208,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -195,8 +248,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -489,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -533,13 +593,27 @@
         <v>6</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="4"/>
+      <c r="B3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -550,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -660,12 +734,192 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="101" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="13"/>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="8">
+        <v>2</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" ht="45">
+      <c r="A10" s="8">
+        <v>3</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" ht="45">
+      <c r="A11" s="8">
+        <v>4</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="8">
+        <v>5</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" ht="30">
+      <c r="A13" s="8">
+        <v>6</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:A5"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C12" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test - user can register ONLY with valid e-mail v.2
</commit_message>
<xml_diff>
--- a/data/ProjekatData.xlsx
+++ b/data/ProjekatData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>Section</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Verify that user can register using only valid email adress</t>
   </si>
   <si>
-    <t>Enter invalid e-mail address</t>
-  </si>
-  <si>
     <t>pera#gmail.com</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>pera@gmail.com</t>
   </si>
   <si>
-    <t>Enter valid e-mail address (for next text enter e-mail in format pera+n@gmail.com…n = 1, 2, 3...)</t>
-  </si>
-  <si>
     <t>TCReg1</t>
   </si>
   <si>
@@ -127,6 +121,21 @@
   </si>
   <si>
     <t>E-mail is accepted, and user is forwarded to "CREATE AN ACCOUNT"</t>
+  </si>
+  <si>
+    <t>Enter invalid e-mail address in "Email address" field</t>
+  </si>
+  <si>
+    <t>Leave "Email address" field empty</t>
+  </si>
+  <si>
+    <t>"Email address" field is empty</t>
+  </si>
+  <si>
+    <t>User can`t registrer with empty "Email address" field. Error message: "Invalid email address." is displayed.</t>
+  </si>
+  <si>
+    <t>Enter valid e-mail address  in "Email address" field(for next text enter e-mail in format pera+n@gmail.com…n = 1, 2, 3...)</t>
   </si>
 </sst>
 </file>
@@ -245,14 +254,14 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -593,7 +602,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>21</v>
@@ -607,9 +616,9 @@
         <v>6</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="4"/>
@@ -665,7 +674,7 @@
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -676,7 +685,7 @@
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="13"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
@@ -734,10 +743,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -765,7 +774,7 @@
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="5"/>
@@ -777,7 +786,7 @@
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -788,7 +797,7 @@
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="13"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
@@ -841,13 +850,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>27</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
@@ -857,68 +866,96 @@
         <v>3</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" ht="45">
+    <row r="11" spans="1:6">
       <c r="A11" s="8">
         <v>4</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="11" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="45">
       <c r="A12" s="8">
         <v>5</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="8" t="s">
         <v>27</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" ht="30">
+    <row r="13" spans="1:6" ht="45">
       <c r="A13" s="8">
         <v>6</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="11" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="25" spans="2:2">
-      <c r="B25" s="3"/>
+    <row r="14" spans="1:6" ht="30">
+      <c r="A14" s="8">
+        <v>7</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:6" ht="30">
+      <c r="A15" s="8">
+        <v>8</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A4:A5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C12" r:id="rId1"/>
+    <hyperlink ref="C14" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Registration tests, valid and invalid e-mail tests are split
</commit_message>
<xml_diff>
--- a/data/ProjekatData.xlsx
+++ b/data/ProjekatData.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="19155" windowHeight="11820" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="19155" windowHeight="11820" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestPlan" sheetId="1" r:id="rId1"/>
     <sheet name="TCReg1" sheetId="2" r:id="rId2"/>
     <sheet name="TCReg2" sheetId="3" r:id="rId3"/>
+    <sheet name="TCReg3" sheetId="5" r:id="rId4"/>
+    <sheet name="TCReg4" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="86">
   <si>
     <t>Section</t>
   </si>
@@ -90,9 +92,6 @@
     <t>TC Reg2</t>
   </si>
   <si>
-    <t>Verify that user can register using only valid email adress</t>
-  </si>
-  <si>
     <t>pera#gmail.com</t>
   </si>
   <si>
@@ -102,15 +101,6 @@
     <t>Click "Create an account button"</t>
   </si>
   <si>
-    <t>User can`t registrer with invalid e-mail. Error message: "Invalid email address." is displayed.</t>
-  </si>
-  <si>
-    <t>Refresh page</t>
-  </si>
-  <si>
-    <t>Page is refreshed, error message is dissapeared. E-mail field is empty and ready for entering an e-mail.</t>
-  </si>
-  <si>
     <t>pera@gmail.com</t>
   </si>
   <si>
@@ -132,10 +122,166 @@
     <t>"Email address" field is empty</t>
   </si>
   <si>
-    <t>User can`t registrer with empty "Email address" field. Error message: "Invalid email address." is displayed.</t>
-  </si>
-  <si>
     <t>Enter valid e-mail address  in "Email address" field(for next text enter e-mail in format pera+n@gmail.com…n = 1, 2, 3...)</t>
+  </si>
+  <si>
+    <t>TCReg3</t>
+  </si>
+  <si>
+    <t>Verify that user can create an account when register with valid e-mail</t>
+  </si>
+  <si>
+    <t>TC Reg3</t>
+  </si>
+  <si>
+    <t>Register with valid e-mail</t>
+  </si>
+  <si>
+    <t>Radio-button "Mr" is selected</t>
+  </si>
+  <si>
+    <t>Petar</t>
+  </si>
+  <si>
+    <t>First name is entered and visible</t>
+  </si>
+  <si>
+    <t>Verify that user have to fill all mandatory fields in order to create an account when register with valid e-mail</t>
+  </si>
+  <si>
+    <t>Petrovic</t>
+  </si>
+  <si>
+    <t>Last name is entered and visible</t>
+  </si>
+  <si>
+    <t>Already entered e-mail is visible in "Email" field</t>
+  </si>
+  <si>
+    <t>Click button "Register"</t>
+  </si>
+  <si>
+    <t>User can`t register with empty mandatory fields. Error message: "There are 6 errors
+You must register at least one phone number.
+passwd is required.
+address1 is required.
+city is required.
+The Zip/Postal code you've entered is invalid. It must follow this format: 00000
+This country requires you to choose a State." is displayed.</t>
+  </si>
+  <si>
+    <t>Enter password in "Password" field</t>
+  </si>
+  <si>
+    <t>Password is entered and represented with dots</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>Date of birth is selected</t>
+  </si>
+  <si>
+    <t>Click radio-button "Mr" in "YOUR PERSONAL INFORMATION" section</t>
+  </si>
+  <si>
+    <t>Enter first name in "First name" field in "YOUR PERSONAL INFORMATION" section</t>
+  </si>
+  <si>
+    <t>Enter last name in "Last name" field in "YOUR PERSONAL INFORMATION" section</t>
+  </si>
+  <si>
+    <t>Check if already entered e-mail is visible in "Email" field in "YOUR PERSONAL INFORMATION" section</t>
+  </si>
+  <si>
+    <t>Check if already entered first name is visible in "First name" field in "YOUR ADDRESS" section</t>
+  </si>
+  <si>
+    <t>Already entered first name is visible in "First name" field</t>
+  </si>
+  <si>
+    <t>Already entered last name is visible in "First name" field</t>
+  </si>
+  <si>
+    <t>Check if already entered last name is visible in "Last name" field in "YOUR ADDRESS" section</t>
+  </si>
+  <si>
+    <t>Enter address in "Address" field in "YOUR ADDRESS" section</t>
+  </si>
+  <si>
+    <t>Vrbina 2</t>
+  </si>
+  <si>
+    <t>Address is entered and visible</t>
+  </si>
+  <si>
+    <t>Select state from "State" dropdown menu</t>
+  </si>
+  <si>
+    <t>Select date of birth in "Date of birth" dropdown-menus</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>Enter city in "City" field in "YOUR ADDRESS" section</t>
+  </si>
+  <si>
+    <t>Honolulu</t>
+  </si>
+  <si>
+    <t>City is entered and visible</t>
+  </si>
+  <si>
+    <t>State is entered and visible</t>
+  </si>
+  <si>
+    <t>Enter postal code in "Zip/Postal Code" field in "YOUR ADDRESS" section</t>
+  </si>
+  <si>
+    <t>Postal code is entered and visible</t>
+  </si>
+  <si>
+    <t>Enter mobile phone number in "Mobile phone" field in "YOUR ADDRESS" section</t>
+  </si>
+  <si>
+    <t>Mobile phone number is entered and visible</t>
+  </si>
+  <si>
+    <t>Enter address alias in "Assign an address alias for future reference"  in "YOUR ADDRESS" section</t>
+  </si>
+  <si>
+    <t>066111222</t>
+  </si>
+  <si>
+    <t>Vrbina</t>
+  </si>
+  <si>
+    <t>Address alias is entered and visible</t>
+  </si>
+  <si>
+    <t>Click "Register" button</t>
+  </si>
+  <si>
+    <t>User is registered and forwarded to "MY ACCOUNT" page</t>
+  </si>
+  <si>
+    <t>Verify that user can register using valid e-mail adress</t>
+  </si>
+  <si>
+    <t>TCReg4</t>
+  </si>
+  <si>
+    <t>Verify that user can`t register using invalid e-mail adress</t>
+  </si>
+  <si>
+    <t>User can`t register with empty "Email address" field. Error message: "Invalid email address." is displayed.</t>
+  </si>
+  <si>
+    <t>User can`t register with invalid e-mail. Error message: "Invalid email address." is displayed.</t>
+  </si>
+  <si>
+    <t>E-mail is accepted, and user is forwarded to "CREATE AN ACCOUNT" page</t>
   </si>
 </sst>
 </file>
@@ -180,7 +326,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -216,6 +362,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -224,7 +394,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -262,6 +432,31 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -558,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -602,7 +797,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>21</v>
@@ -616,13 +811,41 @@
         <v>6</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="4"/>
+      <c r="B4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="4"/>
+      <c r="B5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -743,10 +966,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -775,7 +998,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="C2" s="5"/>
       <c r="E2" s="3"/>
@@ -845,117 +1068,603 @@
       <c r="E8" s="9"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="30">
       <c r="A9" s="8">
         <v>2</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="8" t="s">
+      <c r="B9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:6" ht="45">
+    <row r="10" spans="1:6" ht="30">
       <c r="A10" s="8">
         <v>3</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="11" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="8">
-        <v>4</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" ht="45">
-      <c r="A12" s="8">
-        <v>5</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" ht="45">
-      <c r="A13" s="8">
-        <v>6</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:6" ht="30">
-      <c r="A14" s="8">
-        <v>7</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="1:6" ht="30">
-      <c r="A15" s="8">
-        <v>8</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-    </row>
-    <row r="27" spans="2:2">
-      <c r="B27" s="3"/>
+    <row r="22" spans="2:2">
+      <c r="B22" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A4:A5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C14" r:id="rId1"/>
+    <hyperlink ref="C9" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="101" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="15"/>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="8">
+        <v>2</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" ht="45">
+      <c r="A10" s="8">
+        <v>3</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="8">
+        <v>4</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" ht="45">
+      <c r="A12" s="8">
+        <v>5</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:A5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="101" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" customWidth="1"/>
+    <col min="4" max="4" width="42.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="15"/>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30">
+      <c r="A8" s="8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="8">
+        <v>2</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="8">
+        <v>3</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="8">
+        <v>4</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" ht="30">
+      <c r="A12" s="8">
+        <v>5</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" ht="165">
+      <c r="A13" s="8">
+        <v>6</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="8">
+        <v>7</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="19">
+        <v>8</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="8">
+        <v>1</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="20"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="21"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="4">
+        <v>2000</v>
+      </c>
+      <c r="D17" s="18"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+    </row>
+    <row r="18" spans="1:6" ht="30">
+      <c r="A18" s="22">
+        <v>9</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" ht="30">
+      <c r="A19" s="22">
+        <v>10</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="22">
+        <v>11</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="22">
+        <v>12</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="22">
+        <v>13</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="22">
+        <v>14</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="4">
+        <v>21000</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="22">
+        <v>15</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="22">
+        <v>16</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:6" ht="30">
+      <c r="A26" s="22">
+        <v>17</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="F15:F17"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C12" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
User registartion tests - final
</commit_message>
<xml_diff>
--- a/data/ProjekatData.xlsx
+++ b/data/ProjekatData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="19155" windowHeight="11820" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="19155" windowHeight="11820" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TestPlan" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="TCReg2" sheetId="3" r:id="rId3"/>
     <sheet name="TCReg3" sheetId="5" r:id="rId4"/>
     <sheet name="TCReg4" sheetId="4" r:id="rId5"/>
+    <sheet name="TCReg5" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="91">
   <si>
     <t>Section</t>
   </si>
@@ -266,7 +267,31 @@
     <t>21000</t>
   </si>
   <si>
-    <t>pera+1@gmail.com</t>
+    <t>TCReg5</t>
+  </si>
+  <si>
+    <t>Verify that user cannot register twice with the same email adress</t>
+  </si>
+  <si>
+    <t>TC Reg5</t>
+  </si>
+  <si>
+    <t>User is registered with e-mail:</t>
+  </si>
+  <si>
+    <t>Enter e-mail address in "Email address" field</t>
+  </si>
+  <si>
+    <t>User can`t register twice with the same e-mail address. Error message: "An account using this email address has already been registered. Please enter a valid password or request a new one." is displayed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pera+3@gmail.com</t>
+  </si>
+  <si>
+    <t>pera+4@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pera+4@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -311,7 +336,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -371,6 +396,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -379,7 +417,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -462,6 +500,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -757,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -850,6 +893,20 @@
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="4"/>
+      <c r="B6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -975,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1083,7 +1140,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>24</v>
@@ -1125,7 +1182,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1298,7 +1355,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1451,7 +1508,7 @@
         <v>77</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>24</v>
@@ -1669,4 +1726,160 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="101" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="35"/>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="35"/>
+      <c r="B6" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="8">
+        <v>1</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="8">
+        <v>2</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" ht="75">
+      <c r="A11" s="8">
+        <v>3</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:A6"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Personal information edit test
</commit_message>
<xml_diff>
--- a/data/ProjekatData.xlsx
+++ b/data/ProjekatData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="19155" windowHeight="11820" tabRatio="653"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="19155" windowHeight="11820" tabRatio="653" firstSheet="4" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="TestPlan" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,14 @@
     <sheet name="TCMA1" sheetId="11" r:id="rId11"/>
     <sheet name="TCMA2" sheetId="12" r:id="rId12"/>
     <sheet name="TCMA3" sheetId="13" r:id="rId13"/>
+    <sheet name="TCMA4" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="191">
   <si>
     <t>Section</t>
   </si>
@@ -485,6 +486,120 @@
   </si>
   <si>
     <t>Second address is removed. User is forwarded to "MY ADDRESSES" page. Second address is not visible in "VRBINA" section.</t>
+  </si>
+  <si>
+    <t>TsSu4</t>
+  </si>
+  <si>
+    <t>TCMA4</t>
+  </si>
+  <si>
+    <t>Verify that registered user can update personal informations in "MY ACCOUNT" section</t>
+  </si>
+  <si>
+    <t>Click on "MY PERSONAL INFORMATION" tab</t>
+  </si>
+  <si>
+    <t>User is forwarded to "YOUR PERSONAL INFORMATION" page</t>
+  </si>
+  <si>
+    <t>Click on "Mrs" radio button</t>
+  </si>
+  <si>
+    <t>"Mrs" radio button is selected</t>
+  </si>
+  <si>
+    <t>Click on "First name" field</t>
+  </si>
+  <si>
+    <t>Cursor is visible in "First name" field</t>
+  </si>
+  <si>
+    <t>Delete actual name in "First name" field</t>
+  </si>
+  <si>
+    <t>Actual name is deleted</t>
+  </si>
+  <si>
+    <t>Enter new name in "First name" filed</t>
+  </si>
+  <si>
+    <t>Mara</t>
+  </si>
+  <si>
+    <t>New name in "First name" is entered and visible</t>
+  </si>
+  <si>
+    <t>Click on "Last name" field</t>
+  </si>
+  <si>
+    <t>Cursor is visible in "Last name" field</t>
+  </si>
+  <si>
+    <t>Delete actual last name in "Last name" field</t>
+  </si>
+  <si>
+    <t>Actual last name is deleted</t>
+  </si>
+  <si>
+    <t>Enter new last name in "Last name" filed</t>
+  </si>
+  <si>
+    <t>New last name in "Last name" is entered and visible</t>
+  </si>
+  <si>
+    <t>Days dropdown menu is opened</t>
+  </si>
+  <si>
+    <t>Select day from dropdown menu</t>
+  </si>
+  <si>
+    <t>Day is selected</t>
+  </si>
+  <si>
+    <t>Months dropdown menu is opened</t>
+  </si>
+  <si>
+    <t>Click on days dropdown menu of "Date of birth" section</t>
+  </si>
+  <si>
+    <t>Click on months dropdown menu of "Date of birth" section</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>Month is selected</t>
+  </si>
+  <si>
+    <t>Click on years dropdown menu of "Date of birth" section</t>
+  </si>
+  <si>
+    <t>Years dropdown menu is opened</t>
+  </si>
+  <si>
+    <t>Select year from dropdown menu</t>
+  </si>
+  <si>
+    <t>Select month from dropdown menu</t>
+  </si>
+  <si>
+    <t>Year is selected</t>
+  </si>
+  <si>
+    <t>Click on "Current Password" field</t>
+  </si>
+  <si>
+    <t>Cursor is visible in "Current Password" field</t>
+  </si>
+  <si>
+    <t>Enter valid password</t>
+  </si>
+  <si>
+    <t>User successfully updated personal information. Confirmation message: "Your personal information has been successfully updated." is appeared.</t>
+  </si>
+  <si>
+    <t>Maric</t>
   </si>
 </sst>
 </file>
@@ -1010,10 +1125,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1219,6 +1334,19 @@
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="30">
+      <c r="B14" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1784,8 +1912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1966,6 +2094,384 @@
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:A6"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="101" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="43"/>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="43"/>
+      <c r="B6" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30">
+      <c r="A9" s="8">
+        <v>1</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" ht="30">
+      <c r="A10" s="8">
+        <v>2</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="8">
+        <v>3</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="14">
+        <v>4</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="14">
+        <v>6</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="30">
+      <c r="A14" s="14">
+        <v>7</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="14">
+        <v>8</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="14">
+        <v>9</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" ht="30">
+      <c r="A17" s="14">
+        <v>10</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="14">
+        <v>11</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="14">
+        <v>12</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="C19" s="4">
+        <v>2</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="14">
+        <v>13</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="14">
+        <v>14</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="14">
+        <v>15</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="14">
+        <v>16</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="C23" s="4">
+        <v>1999</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="14">
+        <v>17</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" ht="30">
+      <c r="A25" s="14">
+        <v>18</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:6" ht="60">
+      <c r="A26" s="14">
+        <v>19</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3154,7 +3660,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>